<commit_message>
Update section 3 (first-third paragraphs), section 4.3 memory footprints, section 4.4 threats to validity
Update:
- section 3 (first-third paragraphs)
- section 4.3 memory footprints
- section 4.4 threats to validity
</commit_message>
<xml_diff>
--- a/data/Load Analysis.xlsx
+++ b/data/Load Analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772" tabRatio="827"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772" tabRatio="827" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Conference Load Time" sheetId="32" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>No</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Non-optimised CBP</t>
   </si>
   <si>
-    <t>Non-Optimised CBP</t>
-  </si>
-  <si>
     <t>AVG</t>
   </si>
 </sst>
@@ -88,9 +85,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="0.000000"/>
-    <numFmt numFmtId="170" formatCode="0.0000000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
+    <numFmt numFmtId="167" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -141,15 +138,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2677,7 +2674,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0" l="0" r="0" t="0" header="0" footer="0"/>
-    <c:pageSetup paperSize="9" orientation="landscape"/>
+    <c:pageSetup paperSize="32767" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -8087,7 +8084,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Non-Optimised CBP</c:v>
+                  <c:v>Non-optimised CBP</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -9456,7 +9453,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Non-Optimised CBP</c:v>
+                  <c:v>Non-optimised CBP</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -10475,7 +10472,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Non-Optimised CBP</c:v>
+                  <c:v>Non-optimised CBP</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -12500,6 +12497,1384 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Conference Memory Footprints'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Optimised CBP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="0066CC"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Conference Memory Footprints'!$C$18:$C$67</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>25.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.81</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30.89</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.51</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.869999999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>37.35</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>38.479999999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40.299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41.66</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43.68</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44.97</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>46.48</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>48.47</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>47.96</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>51.07</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>52.73</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>54.16</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>56.21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>57.22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>59.23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>60.63</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>63.17</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>65.290000000000006</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>67.33</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>68.459999999999994</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>69.84</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>71.48</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>75.02</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>76.349999999999994</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>78.09</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>79.78</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>81.38</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>82.24</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>84.4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>85.54</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>86.76</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>88.52</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>90.11</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>91.6</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>93.78</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>94.51</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>95.5</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>98.26</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>99.51</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>100.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Conference Memory Footprints'!$D$18:$D$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>8.395251</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.3124450000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.2478049999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.8318960000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.8431920000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.2754370000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.5957840000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.9200990000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.2988350000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.7439199999999992</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.5234129999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.6104749999999992</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.9387570000000007</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10.153715</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10.435619000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10.806027</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11.137212999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>11.282679999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11.455704000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11.816629000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>12.288845</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>12.293949</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>12.778703999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>12.905195000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12.922565000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>13.427562999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>13.371162999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>14.143179</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>14.13232</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>14.443759999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>14.822260999999999</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>15.099443000000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>15.551507000000001</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>15.633063999999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>16.137132999999999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>16.344546999999999</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>16.877559999999999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>17.179576000000001</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>17.422682999999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>17.490114999999999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>17.830127999999998</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>17.853155000000001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>18.197845000000001</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>18.259786999999999</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>18.541188999999999</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>19.035</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>18.899539000000001</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>19.595443</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>19.85472</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>20.066320000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A84A-470F-8E73-DBCE1583B78D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Conference Memory Footprints'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Non-optimised CBP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Conference Memory Footprints'!$C$18:$C$67</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>25.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.81</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30.89</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.51</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.869999999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>37.35</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>38.479999999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40.299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41.66</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43.68</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44.97</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>46.48</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>48.47</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>47.96</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>51.07</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>52.73</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>54.16</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>56.21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>57.22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>59.23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>60.63</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>63.17</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>65.290000000000006</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>67.33</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>68.459999999999994</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>69.84</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>71.48</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>75.02</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>76.349999999999994</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>78.09</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>79.78</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>81.38</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>82.24</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>84.4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>85.54</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>86.76</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>88.52</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>90.11</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>91.6</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>93.78</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>94.51</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>95.5</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>98.26</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>99.51</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>100.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Conference Memory Footprints'!$E$18:$E$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>4.8404749999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.8870610000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5985230000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.7587839999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.689981</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.8503069999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.1201040000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.2547870000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.4018350000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.6911360000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.2787649999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.1715949999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.2497870000000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.3112349999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.3613090000000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.5102130000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.5619550000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.6460429999999997</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.6082239999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.7983549999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.9289329999999998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.883451</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.0597969999999997</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.047256</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.8908829999999996</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.2086240000000004</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.931133</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.3301629999999998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.2150030000000003</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.3307549999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.5250640000000004</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.668939</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.7552909999999997</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.6785439999999996</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6.007117</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5.9312110000000002</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>6.3119730000000001</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>6.4181359999999996</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>6.4251230000000001</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>6.4513230000000004</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>6.6812849999999999</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>6.3724910000000001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>6.490888</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>6.2923330000000002</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>6.3549090000000001</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>6.6621680000000003</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>6.4253439999999999</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>6.7360879999999996</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>6.8444450000000003</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>6.9207789999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A84A-470F-8E73-DBCE1583B78D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Conference Memory Footprints'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>XMI</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="008000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Conference Memory Footprints'!$C$18:$C$67</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>25.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.81</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30.89</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.51</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.869999999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>37.35</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>38.479999999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40.299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41.66</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43.68</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44.97</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>46.48</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>48.47</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>47.96</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>51.07</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>52.73</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>54.16</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>56.21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>57.22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>59.23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>60.63</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>63.17</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>65.290000000000006</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>67.33</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>68.459999999999994</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>69.84</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>71.48</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>75.02</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>76.349999999999994</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>78.09</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>79.78</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>81.38</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>82.24</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>84.4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>85.54</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>86.76</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>88.52</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>90.11</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>91.6</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>93.78</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>94.51</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>95.5</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>98.26</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>99.51</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>100.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Conference Memory Footprints'!$F$18:$F$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>5.4694430000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1046529999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.7673810000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.3366049999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.059971</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.6260750000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.8939249999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.7126109999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.6449250000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.7273969999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.7486269999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.7672159999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.8318319999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.8180640000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.8318989999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.014507</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.922949</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.9112290000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.9185680000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.9781840000000002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.0415869999999998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.2285599999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.0641280000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.1947869999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.3672399999999998</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.3726130000000003</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.4867650000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.4037920000000002</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.5143969999999998</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.5149759999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.7936129999999997</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.588781</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.8269330000000004</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.2723120000000003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.9140160000000002</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5.2441170000000001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.1594800000000003</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.5895200000000003</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>5.1944990000000004</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>5.1551629999999999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5.7179789999999997</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.5167729999999997</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.5742770000000004</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.585763</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.5285890000000002</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.5463870000000002</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.533563</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.672288</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.6689889999999998</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.6979949999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A84A-470F-8E73-DBCE1583B78D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="360758984"/>
+        <c:axId val="360755704"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="360758984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="cmr10" panose="020B0500000000000000" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="Linux Biolinum" panose="02000503000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="Linux Biolinum" panose="02000503000000000000" pitchFamily="2" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number of Elements (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>×100)</a:t>
+                </a:r>
+                <a:endParaRPr lang="id-ID"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="cmr10" panose="020B0500000000000000" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="Linux Biolinum" panose="02000503000000000000" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="Linux Biolinum" panose="02000503000000000000" pitchFamily="2" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="id-ID"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="cmr10" panose="020B0500000000000000" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Linux Biolinum" panose="02000503000000000000" pitchFamily="2" charset="0"/>
+                <a:cs typeface="Linux Biolinum" panose="02000503000000000000" pitchFamily="2" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="id-ID"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="360755704"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="360755704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="21"/>
+          <c:min val="3"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="cmr10" panose="020B0500000000000000" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="Linux Biolinum" panose="02000503000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="Linux Biolinum" panose="02000503000000000000" pitchFamily="2" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Memory Size (MB)</a:t>
+                </a:r>
+                <a:endParaRPr lang="id-ID"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.5434027777777777E-2"/>
+              <c:y val="0.1366512219321652"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="cmr10" panose="020B0500000000000000" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="Linux Biolinum" panose="02000503000000000000" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="Linux Biolinum" panose="02000503000000000000" pitchFamily="2" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="id-ID"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="cmr10" panose="020B0500000000000000" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Linux Biolinum" panose="02000503000000000000" pitchFamily="2" charset="0"/>
+                <a:cs typeface="Linux Biolinum" panose="02000503000000000000" pitchFamily="2" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="id-ID"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="360758984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="cmr10" panose="020B0500000000000000" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Linux Biolinum" panose="02000503000000000000" pitchFamily="2" charset="0"/>
+              <a:cs typeface="Linux Biolinum" panose="02000503000000000000" pitchFamily="2" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="id-ID"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1000" b="0">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:latin typeface="cmr10" panose="020B0500000000000000" pitchFamily="34" charset="0"/>
+          <a:ea typeface="Linux Biolinum" panose="02000503000000000000" pitchFamily="2" charset="0"/>
+          <a:cs typeface="Linux Biolinum" panose="02000503000000000000" pitchFamily="2" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="id-ID"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0" l="0" r="0" t="0" header="0" footer="0"/>
+    <c:pageSetup paperSize="32767" orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -12781,6 +14156,46 @@
 </file>
 
 <file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -16948,6 +18363,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -17264,6 +19195,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>486960</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>34060</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D91C4DF-3D26-406E-8A81-5A525E81C6CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -17566,8 +19535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21014,10 +22983,10 @@
     <row r="71" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D71" s="10"/>
       <c r="E71" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F71" s="10">
-        <f t="shared" ref="E71:H71" si="9">AVERAGE(F2:F70)</f>
+        <f t="shared" ref="F71:H71" si="9">AVERAGE(F2:F70)</f>
         <v>8.4217391304347855E-2</v>
       </c>
       <c r="G71" s="10">
@@ -21029,7 +22998,7 @@
         <v>1.6702463768115945</v>
       </c>
       <c r="J71" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K71" s="5">
         <f>AVERAGE(K2:K70)</f>
@@ -25650,7 +27619,7 @@
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C219" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D219" s="9">
         <f>AVERAGE(D2:D218)</f>
@@ -25676,9 +27645,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25702,7 +27671,7 @@
         <v>14</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>13</v>
@@ -27096,7 +29065,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C68" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D68" s="11">
         <f>AVERAGE(D2:D67)</f>

</xml_diff>

<commit_message>
Fix typos and punctuation
Fix typos and punctuation
</commit_message>
<xml_diff>
--- a/data/Load Analysis.xlsx
+++ b/data/Load Analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772" tabRatio="827" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772" tabRatio="827" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Conference Load Time" sheetId="32" r:id="rId1"/>
@@ -5545,7 +5545,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Append Time (miliseconds)</a:t>
+                  <a:t>Append Time (milliseconds)</a:t>
                 </a:r>
                 <a:endParaRPr lang="id-ID"/>
               </a:p>
@@ -7908,7 +7908,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Append Time (miliseconds)</a:t>
+                  <a:t>Append Time (milliseconds)</a:t>
                 </a:r>
                 <a:endParaRPr lang="id-ID"/>
               </a:p>
@@ -23028,8 +23028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F219"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27645,8 +27645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>